<commit_message>
all modification are done on the both testcases
</commit_message>
<xml_diff>
--- a/AvionSchoolLMSGUIFramework/testdata/Avion_School_Test_Script_Data.xlsx
+++ b/AvionSchoolLMSGUIFramework/testdata/Avion_School_Test_Script_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="3000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="3000"/>
   </bookViews>
   <sheets>
     <sheet name="Admin_messaging" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K8"/>
 </workbook>
 </file>
 
@@ -130,13 +131,13 @@
     <t>harireddy</t>
   </si>
   <si>
-    <t>virat</t>
-  </si>
-  <si>
-    <t>hi virat how are you</t>
-  </si>
-  <si>
     <t>reddy</t>
+  </si>
+  <si>
+    <t>ronaldo</t>
+  </si>
+  <si>
+    <t>hi ronaldo how are you</t>
   </si>
 </sst>
 </file>
@@ -532,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,10 +570,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>8</v>
@@ -643,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +708,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>35</v>

</xml_diff>